<commit_message>
nach Anmerkungen von Robert zu Diagrammen
</commit_message>
<xml_diff>
--- a/Grafiken_Pool/Datenreihen/Simu/DeliveryRatio_1-80.xlsx
+++ b/Grafiken_Pool/Datenreihen/Simu/DeliveryRatio_1-80.xlsx
@@ -34,7 +34,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="1-80_OPT_recCnt-1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/Jens/Dropbox/UNI Jens/Masterarbeit/Thesis/Grafiken_Pool/Datenreihen/Simu/1-80_OPT_recCnt-1.csv" decimal="," thousands="." tab="0" comma="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="/Users/Jens/Dropbox/UNI Jens/Masterarbeit/Thesis/Grafiken_Pool/Datenreihen/Simu/1-80_OPT_recCnt-1.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="41">
         <textField/>
         <textField/>
@@ -81,7 +81,7 @@
     </textPr>
   </connection>
   <connection id="2" name="1-80_STD_recCnt-1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/Jens/Dropbox/UNI Jens/Masterarbeit/Thesis/Grafiken_Pool/Datenreihen/Simu/1-80_STD_recCnt-1.csv" decimal="," thousands="." tab="0" comma="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="/Users/Jens/Dropbox/UNI Jens/Masterarbeit/Thesis/Grafiken_Pool/Datenreihen/Simu/1-80_STD_recCnt-1.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="41">
         <textField/>
         <textField/>
@@ -301,9 +301,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -581,10 +579,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -862,11 +857,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="342814096"/>
-        <c:axId val="342819024"/>
+        <c:axId val="-1999809728"/>
+        <c:axId val="-2038248624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="342814096"/>
+        <c:axId val="-1999809728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,6 +881,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1800"/>
+                  <a:t>Anzahl der gleichzeitig antwortenden Frachtcontainer</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -904,11 +955,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -923,16 +974,16 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342819024"/>
+        <c:crossAx val="-2038248624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:tickLblSkip val="1"/>
+        <c:tickLblSkip val="3"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="342819024"/>
+        <c:axId val="-2038248624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -953,6 +1004,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1800"/>
+                  <a:t>Product Specific Delivery Ratio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -969,7 +1076,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -984,7 +1091,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342814096"/>
+        <c:crossAx val="-1999809728"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1002,9 +1109,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.871432024076169"/>
-          <c:y val="0.435034234851078"/>
-          <c:w val="0.104553837860732"/>
+          <c:x val="0.810754222222222"/>
+          <c:y val="0.291403373015873"/>
+          <c:w val="0.151120555555556"/>
           <c:h val="0.154776250794738"/>
         </c:manualLayout>
       </c:layout>
@@ -1021,7 +1128,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1046,12 +1153,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1637,10 +1739,10 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>173500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>74300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1663,7 +1765,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1-80_OPT_recCnt-1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="10-400_OPT_recCnt-1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1671,7 +1773,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="10-400_OPT_recCnt-1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1-80_OPT_recCnt-1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1939,8 +2041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AP6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AR18" sqref="AR18"/>
+    <sheetView tabSelected="1" topLeftCell="L4" workbookViewId="0">
+      <selection activeCell="AO15" sqref="AO15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2374,7 +2476,7 @@
         <v>0.87666666666666671</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="D5:AP6" si="1">E2/(E$1*100)</f>
+        <f t="shared" ref="E5:AP5" si="1">E2/(E$1*100)</f>
         <v>0.79200000000000004</v>
       </c>
       <c r="F5">

</xml_diff>